<commit_message>
Heatsink updated to 12x12x12mm w/ tape
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM v0.2b BOM.xlsx
+++ b/PCB/v0.2 archive/TeensyROM v0.2b BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E257A1AA-F4D7-4363-87BA-95D8B14A624A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7EB73D-B6F3-491E-99DB-15BFA1D5006C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
+    <workbookView xWindow="3690" yWindow="-15060" windowWidth="23370" windowHeight="13710" xr2:uid="{5596D14A-B5AE-4503-9066-038068479CCD}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'0.2 Export'!$A$1:$O$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$J$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$J$27</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="207">
   <si>
     <t>Value</t>
   </si>
@@ -443,9 +443,6 @@
   </si>
   <si>
     <t>U1 Heatsink</t>
-  </si>
-  <si>
-    <t>14x14mm Aluminum heatsink w/ Thermal Conductive Adhesive Tape</t>
   </si>
   <si>
     <t>Optional, but recommended</t>
@@ -609,9 +606,6 @@
     </r>
   </si>
   <si>
-    <t>2223-HSB03-141406-ND</t>
-  </si>
-  <si>
     <t>Multiple subs, such as these w/ thermal tape attached</t>
   </si>
   <si>
@@ -695,11 +689,33 @@
     <t>For Teensy Ethernet connection to TeensyROM.</t>
   </si>
   <si>
-    <t>CUI Devices HSB03-141406 (+ therm tape or glue)</t>
-  </si>
-  <si>
     <t>2 layer board: 2.40 x 2.70 x 0.063 inches
 Recommend ENIG finish, 30° chamfered gold fingers, Purple solder mask</t>
+  </si>
+  <si>
+    <t>AE11386-ND</t>
+  </si>
+  <si>
+    <t>U1 Therm Pad</t>
+  </si>
+  <si>
+    <t>11x11mm Thermal Conductive Adhesive Tape</t>
+  </si>
+  <si>
+    <t>t-Global
+TG-T1000-11-11-0.25-5PT</t>
+  </si>
+  <si>
+    <t>Assmann V2019B</t>
+  </si>
+  <si>
+    <t>1168-TG-T1000-11-11-0.25-5PT-ND</t>
+  </si>
+  <si>
+    <t>16a</t>
+  </si>
+  <si>
+    <t>12x12mm Aluminum heatsink</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1325,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1323,7 +1339,7 @@
     <col min="4" max="4" width="33.109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="26.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="23.21875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="23.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="7" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5546875" style="19" customWidth="1"/>
     <col min="10" max="10" width="35.77734375" style="7" customWidth="1"/>
@@ -1338,7 +1354,7 @@
         <v>18</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>0</v>
@@ -1347,16 +1363,16 @@
         <v>30</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>25</v>
@@ -1376,13 +1392,13 @@
         <v>107</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H2" s="21">
         <f>32.4/3</f>
@@ -1393,7 +1409,7 @@
         <v>10.799999999999999</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1404,19 +1420,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>138</v>
       </c>
       <c r="H3" s="21">
         <v>0.1</v>
@@ -1435,19 +1451,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>179</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>181</v>
       </c>
       <c r="H4" s="21">
         <v>0.1</v>
@@ -1466,19 +1482,19 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="25" t="s">
         <v>148</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>149</v>
       </c>
       <c r="H5" s="22">
         <v>0.1</v>
@@ -1500,7 +1516,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>108</v>
@@ -1519,7 +1535,7 @@
         <v>2.72</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="28.8">
@@ -1533,16 +1549,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F7" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>184</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>186</v>
       </c>
       <c r="H7" s="21">
         <v>0.5</v>
@@ -1552,7 +1568,7 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="43.2">
@@ -1569,13 +1585,13 @@
         <v>124</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F8" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H8" s="21">
         <v>33.08</v>
@@ -1585,7 +1601,7 @@
         <v>33.08</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="28.8">
@@ -1599,16 +1615,16 @@
         <v>105</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>161</v>
-      </c>
       <c r="G9" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H9" s="21">
         <v>1.31</v>
@@ -1632,16 +1648,16 @@
         <v>104</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>165</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>166</v>
       </c>
       <c r="H10" s="21">
         <v>0.26</v>
@@ -1651,7 +1667,7 @@
         <v>0.26</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8">
@@ -1665,13 +1681,13 @@
         <v>106</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>112</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>39</v>
@@ -1684,7 +1700,7 @@
         <v>0.19</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1698,7 +1714,7 @@
         <v>43</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>32</v>
@@ -1713,7 +1729,7 @@
         <v>0.19</v>
       </c>
       <c r="I12" s="21">
-        <f t="shared" ref="I12:I17" si="2">H12*B12</f>
+        <f t="shared" ref="I12:I18" si="2">H12*B12</f>
         <v>0.19</v>
       </c>
       <c r="J12" s="6"/>
@@ -1748,7 +1764,7 @@
         <v>0.43</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8">
@@ -1762,16 +1778,16 @@
         <v>20</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H14" s="21">
         <v>0.22</v>
@@ -1781,7 +1797,7 @@
         <v>0.44</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1850,7 +1866,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="28.8" customHeight="1">
+    <row r="17" spans="1:10" ht="28.8">
       <c r="A17" s="16">
         <v>16</v>
       </c>
@@ -1861,62 +1877,71 @@
         <v>131</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="H17" s="21">
         <v>0.74</v>
       </c>
       <c r="I17" s="21">
+        <f>H17*B17</f>
+        <v>0.74</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="28.8">
+      <c r="A18" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="H18" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="I18" s="21">
         <f t="shared" si="2"/>
-        <v>0.74</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A18" s="45">
-        <v>17</v>
-      </c>
-      <c r="B18" s="36">
-        <v>2</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="36" t="s">
-        <v>192</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A19" s="45">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
@@ -1924,131 +1949,131 @@
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
       <c r="J19" s="36" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A20" s="45">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="36">
         <v>1</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>114</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
       <c r="J20" s="36" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A21" s="45">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="36">
         <v>1</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="E21" s="39" t="s">
-        <v>153</v>
+        <v>111</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>112</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="36"/>
+        <v>113</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>114</v>
+      </c>
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
       <c r="J21" s="36" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A22" s="45">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="36">
         <v>1</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>125</v>
+        <v>194</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F22" s="36" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
       <c r="J22" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:10" hidden="1" outlineLevel="1">
-      <c r="A23" s="44">
-        <v>22</v>
-      </c>
-      <c r="B23" s="40">
-        <v>1</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>145</v>
-      </c>
-      <c r="E23" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="41" t="s">
-        <v>116</v>
+      <c r="A23" s="45">
+        <v>21</v>
+      </c>
+      <c r="B23" s="36">
+        <v>1</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="36" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A24" s="44">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="40">
         <v>1</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="E24" s="41"/>
+        <v>72</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>103</v>
+      </c>
       <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
+      <c r="G24" s="41" t="s">
+        <v>26</v>
+      </c>
       <c r="H24" s="42"/>
       <c r="I24" s="42"/>
       <c r="J24" s="41" t="s">
@@ -2057,16 +2082,16 @@
     </row>
     <row r="25" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A25" s="44">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="40">
         <v>1</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="41" t="s">
-        <v>146</v>
+        <v>84</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>118</v>
       </c>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
@@ -2074,21 +2099,21 @@
       <c r="H25" s="42"/>
       <c r="I25" s="42"/>
       <c r="J25" s="41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:10" hidden="1" outlineLevel="1">
       <c r="A26" s="44">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="40">
         <v>1</v>
       </c>
       <c r="C26" s="41" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="E26" s="41"/>
       <c r="F26" s="41"/>
@@ -2099,80 +2124,102 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="31" customFormat="1" ht="13.8" customHeight="1" collapsed="1">
-      <c r="A27" s="46"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="32"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="H28" s="20" t="s">
+    <row r="27" spans="1:10" hidden="1" outlineLevel="1">
+      <c r="A27" s="44">
+        <v>25</v>
+      </c>
+      <c r="B27" s="40">
+        <v>1</v>
+      </c>
+      <c r="C27" s="41" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="31" customFormat="1" ht="13.8" customHeight="1" collapsed="1">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="32"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="H29" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="I29" s="29">
+        <f>SUM(I2:I27)</f>
+        <v>58.459999999999994</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="H30" s="33" t="s">
+        <v>167</v>
+      </c>
+      <c r="I30" s="19">
+        <f>I29*10%</f>
+        <v>5.8460000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="H31" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="I31" s="24">
+        <f>I30+I29</f>
+        <v>64.305999999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="H32" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="I32" s="19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9">
+      <c r="G33" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="I28" s="29">
-        <f>SUM(I2:I26)</f>
-        <v>58.259999999999991</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="H29" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="I29" s="19">
-        <f>I28*10%</f>
-        <v>5.8259999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="H30" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="I30" s="24">
-        <f>I29+I28</f>
-        <v>64.085999999999984</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="H31" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="I31" s="19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="G32" s="48" t="s">
+      <c r="H33" s="48"/>
+      <c r="I33" s="24">
+        <f>I32+I31</f>
+        <v>79.305999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9">
+      <c r="G34" s="30"/>
+      <c r="H34" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="H32" s="48"/>
-      <c r="I32" s="24">
-        <f>I31+I30</f>
-        <v>79.085999999999984</v>
-      </c>
-    </row>
-    <row r="33" spans="7:9">
-      <c r="G33" s="30"/>
-      <c r="H33" s="23" t="s">
+      <c r="I34" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="I33" s="23" t="s">
-        <v>173</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J26" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}"/>
+  <autoFilter ref="A1:J27" xr:uid="{AF206551-7640-46D5-B880-F3B0BFEA8EA5}"/>
   <mergeCells count="1">
-    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E8" r:id="rId1" display="https://www.pjrc.com/store" xr:uid="{134792E2-B64E-4FBB-BFC7-EC447106886D}"/>
-    <hyperlink ref="E17" r:id="rId2" display="Multiple, such as: https://www.amazon.com/Heatsink-14x14x10mm-0-55x0-55x0-39-Conductive-Dissipation/dp/B07ZC68LNM/" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
+    <hyperlink ref="E17" r:id="rId2" xr:uid="{5FD644F6-19A2-4D0C-BDC2-C003DADB325A}"/>
     <hyperlink ref="G6" r:id="rId3" display="https://www.digikey.com/en/products/detail/nexperia-usa-inc/74LVC245AD-118/946690" xr:uid="{58DCABB5-EDC7-4E2D-A244-D34D14A1826B}"/>
     <hyperlink ref="F8" r:id="rId4" xr:uid="{8F740FC1-EDF0-4C9E-9823-C987C0E04A4F}"/>
     <hyperlink ref="G8" r:id="rId5" xr:uid="{0DE6FCC4-E35A-47FB-9DC7-F030B4E296C0}"/>
@@ -2189,11 +2236,13 @@
     <hyperlink ref="G10" r:id="rId16" xr:uid="{DF130F23-5B34-41D1-86C6-D27E2C2FCFE8}"/>
     <hyperlink ref="G17" r:id="rId17" xr:uid="{E52F636D-3699-4616-A972-2410D7682974}"/>
     <hyperlink ref="G4" r:id="rId18" xr:uid="{BFF33686-00DA-47D6-B57E-31FEFD3C8B56}"/>
-    <hyperlink ref="E21" r:id="rId19" display="https://www.pjrc.com/store" xr:uid="{4CF63453-125C-408F-8E09-8A412D6E1A65}"/>
-    <hyperlink ref="E22" r:id="rId20" display="https://www.pjrc.com/store" xr:uid="{AFCDA104-AF2B-4C61-8019-A6A0C8B60F5C}"/>
+    <hyperlink ref="E22" r:id="rId19" display="https://www.pjrc.com/store" xr:uid="{4CF63453-125C-408F-8E09-8A412D6E1A65}"/>
+    <hyperlink ref="E23" r:id="rId20" display="https://www.pjrc.com/store" xr:uid="{AFCDA104-AF2B-4C61-8019-A6A0C8B60F5C}"/>
+    <hyperlink ref="E18" r:id="rId21" xr:uid="{90126B75-8BEB-424E-8FE0-DEBACDA6E296}"/>
+    <hyperlink ref="G18" r:id="rId22" display="https://www.digikey.com/en/products/detail/t-global-technology/TG-T1000-11-11-0-25-5PT/13919490" xr:uid="{2859B1F5-9DA9-47E4-8E21-91710442DAD7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
 

</xml_diff>